<commit_message>
Redistribution de la Roadmap + Renomées d'espèce (début)
</commit_message>
<xml_diff>
--- a/Les différents types de Ferae.xlsx
+++ b/Les différents types de Ferae.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X181880\OneDrive - GROUP DIGITAL WORKPLACE\Documents\Privé\Ferae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bertolen\Documents\JdR\Univers\Chroniques des Ténèbres\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FD72BB3F-1182-489A-AF03-63ACBC7C59A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{A2D074A1-80A0-4B01-B3A3-B9DF93BE700D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60972353-64A2-401E-B1B4-5C2C8C4A198F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Espèces" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Auspices!$A$1:$G$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Espèces!$A$1:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Espèces!$A$1:$L$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tribus!$A$1:$B$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="186">
   <si>
     <t>Espèce</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t>Mort</t>
+  </si>
+  <si>
+    <t>Renomée</t>
   </si>
 </sst>
 </file>
@@ -961,28 +964,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="37.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.73046875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,26 +1001,29 @@
       <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1033,14 +1039,14 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1056,11 +1062,11 @@
       <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1076,20 +1082,23 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>184</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>182</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1105,17 +1114,17 @@
       <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1131,11 +1140,11 @@
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1151,9 +1160,9 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1169,14 +1178,14 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1209,17 +1218,20 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="L10" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1235,14 +1247,14 @@
       <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1258,14 +1270,14 @@
       <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>165</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="L12" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1281,29 +1293,32 @@
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>146</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I14" s="4"/>
       <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K13" xr:uid="{34298D81-0FE3-402E-ACB8-ACB4A3B717C7}">
+  <autoFilter ref="A1:L13" xr:uid="{34298D81-0FE3-402E-ACB8-ACB4A3B717C7}">
     <filterColumn colId="1">
       <filters>
         <filter val="Luna"/>
@@ -1324,12 +1339,12 @@
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1343,7 +1358,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1351,7 +1366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1374,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1375,7 +1390,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1398,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1391,7 +1406,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1399,7 +1414,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1407,7 +1422,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1415,7 +1430,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1431,7 +1446,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1439,7 +1454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1473,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1469,7 +1484,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1480,7 +1495,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1491,7 +1506,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1502,7 +1517,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1513,7 +1528,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1524,7 +1539,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1535,7 +1550,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1543,7 +1558,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1559,7 +1574,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1575,7 +1590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1583,7 +1598,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1591,7 +1606,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1607,7 +1622,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1615,7 +1630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1623,7 +1638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1631,7 +1646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1639,7 +1654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1655,7 +1670,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1663,7 +1678,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1671,7 +1686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1679,7 +1694,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -1687,7 +1702,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1695,7 +1710,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -1718,18 +1733,18 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="73.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" customWidth="1"/>
+    <col min="5" max="5" width="73.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1755,7 +1770,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1781,7 +1796,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1833,7 +1848,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1859,7 +1874,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1885,7 +1900,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1905,7 +1920,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1945,7 +1960,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1965,7 +1980,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1987,7 +2002,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -2009,7 +2024,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2031,7 +2046,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2068,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2090,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2112,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2117,7 +2132,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2137,7 +2152,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Ajout de la colonne Archétypes
</commit_message>
<xml_diff>
--- a/Les différents types de Ferae.xlsx
+++ b/Les différents types de Ferae.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X181880\OneDrive - GROUP DIGITAL WORKPLACE\Documents\Privé\Ferae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bertolen\Documents\JdR\Univers\Chroniques des Ténèbres\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="866" documentId="6_{0B842FC3-04D2-4DB4-832A-0232CD8B1350}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{05234578-F408-40FF-B4F6-25F2BC260D79}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC3EF67-1937-4786-9059-44D112726FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="2520" windowWidth="15375" windowHeight="8460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Espèces" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Auspices!$A$1:$G$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Espèces!$A$1:$L$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Espèces!$A$1:$M$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Formes!$A$1:$G$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Formes (2)'!$A$1:$H$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tribus!$A$1:$B$43</definedName>
@@ -34,7 +34,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="257">
   <si>
     <t>Espèce</t>
   </si>
@@ -1774,6 +1776,36 @@
 Griffes et crocs +0L
 Ne provoque pas la Lunacie</t>
     </r>
+  </si>
+  <si>
+    <t>Archétype</t>
+  </si>
+  <si>
+    <t>Comploteur</t>
+  </si>
+  <si>
+    <t>Érudit</t>
+  </si>
+  <si>
+    <t>Messager</t>
+  </si>
+  <si>
+    <t>Guerrisseur</t>
+  </si>
+  <si>
+    <t>Mémoire</t>
+  </si>
+  <si>
+    <t>Assassin</t>
+  </si>
+  <si>
+    <t>Farceur</t>
+  </si>
+  <si>
+    <t>Traqueur</t>
+  </si>
+  <si>
+    <t>Manipulateur</t>
   </si>
 </sst>
 </file>
@@ -2037,7 +2069,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9517,7 +9549,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529768672"/>
@@ -9576,7 +9608,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529138424"/>
@@ -9628,7 +9660,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9665,7 +9697,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10523,28 +10555,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.59765625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.73046875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10555,34 +10588,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10592,20 +10628,20 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10615,17 +10651,20 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -10635,29 +10674,32 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>184</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>182</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -10667,23 +10709,26 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -10693,17 +10738,20 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -10713,20 +10761,23 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>186</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -10736,20 +10787,23 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -10759,14 +10813,17 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -10776,26 +10833,29 @@
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="M10" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -10805,20 +10865,20 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -10828,20 +10888,20 @@
       <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>21</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>165</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="M12" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -10851,43 +10911,46 @@
       <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E13">
         <v>8</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>138</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>146</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J14" s="4"/>
       <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>187</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L13" xr:uid="{34298D81-0FE3-402E-ACB8-ACB4A3B717C7}"/>
+  <autoFilter ref="A1:M13" xr:uid="{34298D81-0FE3-402E-ACB8-ACB4A3B717C7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -10902,12 +10965,12 @@
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10921,7 +10984,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -10929,7 +10992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -10937,7 +11000,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -10945,7 +11008,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -10953,7 +11016,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10961,7 +11024,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -10969,7 +11032,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -10977,7 +11040,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -10985,7 +11048,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -10993,7 +11056,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -11001,7 +11064,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -11009,7 +11072,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -11017,7 +11080,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -11025,7 +11088,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -11036,7 +11099,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -11047,7 +11110,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -11058,7 +11121,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -11069,7 +11132,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -11080,7 +11143,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -11091,7 +11154,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -11102,7 +11165,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -11113,7 +11176,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -11121,7 +11184,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -11129,7 +11192,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -11137,7 +11200,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -11145,7 +11208,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -11153,7 +11216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -11161,7 +11224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -11169,7 +11232,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -11177,7 +11240,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -11185,7 +11248,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -11193,7 +11256,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -11201,7 +11264,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -11209,7 +11272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -11217,7 +11280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -11225,7 +11288,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -11233,7 +11296,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -11241,7 +11304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -11249,7 +11312,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -11257,7 +11320,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -11265,7 +11328,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -11273,7 +11336,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -11296,18 +11359,18 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="73.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" customWidth="1"/>
+    <col min="5" max="5" width="73.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -11333,7 +11396,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -11359,7 +11422,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -11385,7 +11448,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -11411,7 +11474,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -11437,7 +11500,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -11463,7 +11526,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -11483,7 +11546,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -11503,7 +11566,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -11523,7 +11586,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -11543,7 +11606,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -11565,7 +11628,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -11587,7 +11650,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -11609,7 +11672,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -11631,7 +11694,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -11653,7 +11716,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -11675,7 +11738,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -11695,7 +11758,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -11715,7 +11778,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -11747,22 +11810,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC9E6D6-F6D2-4E02-9E27-2D34B665D87B}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="7" max="7" width="15.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11785,7 +11848,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -11806,7 +11869,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
@@ -11827,7 +11890,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -11848,7 +11911,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -11869,7 +11932,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -11890,7 +11953,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="156.75" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
@@ -11913,7 +11976,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -11934,7 +11997,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
@@ -11955,7 +12018,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>24</v>
       </c>
@@ -11976,7 +12039,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>26</v>
       </c>
@@ -11997,7 +12060,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>28</v>
       </c>
@@ -12018,7 +12081,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="228" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>30</v>
       </c>
@@ -12041,17 +12104,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="3:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" ht="57" x14ac:dyDescent="0.45">
       <c r="C19" s="7" t="s">
         <v>237</v>
       </c>
@@ -12075,17 +12138,17 @@
       <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12111,7 +12174,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
@@ -12138,7 +12201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -12165,7 +12228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -12192,7 +12255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>3</v>
       </c>
@@ -12219,7 +12282,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
@@ -12251,7 +12314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>3</v>
       </c>
@@ -12283,7 +12346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
@@ -12310,7 +12373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="19" t="s">
         <v>6</v>
       </c>
@@ -12333,7 +12396,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>6</v>
       </c>
@@ -12356,7 +12419,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
         <v>6</v>
       </c>
@@ -12379,7 +12442,7 @@
       </c>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
@@ -12402,7 +12465,7 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>6</v>
       </c>
@@ -12419,7 +12482,7 @@
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21">
-        <f t="shared" ref="E13:H13" si="3">F9+F10+F15-$D15</f>
+        <f t="shared" ref="F13:H13" si="3">F9+F10+F15-$D15</f>
         <v>5</v>
       </c>
       <c r="G13" s="21">
@@ -12431,7 +12494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>6</v>
       </c>
@@ -12448,7 +12511,7 @@
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="21">
-        <f t="shared" ref="E14:H14" si="4">F10</f>
+        <f t="shared" ref="F14:H14" si="4">F10</f>
         <v>3</v>
       </c>
       <c r="G14" s="21">
@@ -12460,7 +12523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
         <v>6</v>
       </c>
@@ -12485,7 +12548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="23" t="s">
         <v>10</v>
       </c>
@@ -12512,7 +12575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="23" t="s">
         <v>10</v>
       </c>
@@ -12539,7 +12602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="23" t="s">
         <v>10</v>
       </c>
@@ -12566,7 +12629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="23" t="s">
         <v>10</v>
       </c>
@@ -12593,7 +12656,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>10</v>
       </c>
@@ -12625,7 +12688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="23" t="s">
         <v>10</v>
       </c>
@@ -12657,7 +12720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="23" t="s">
         <v>10</v>
       </c>
@@ -12684,7 +12747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>12</v>
       </c>
@@ -12707,7 +12770,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="27" t="s">
         <v>12</v>
       </c>
@@ -12730,7 +12793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>12</v>
       </c>
@@ -12753,7 +12816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="27" t="s">
         <v>12</v>
       </c>
@@ -12776,7 +12839,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="27" t="s">
         <v>12</v>
       </c>
@@ -12793,7 +12856,7 @@
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="29">
-        <f t="shared" ref="E27:H27" si="7">F23+F24+F29-$D29</f>
+        <f t="shared" ref="F27:H27" si="7">F23+F24+F29-$D29</f>
         <v>2</v>
       </c>
       <c r="G27" s="29"/>
@@ -12802,7 +12865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="27" t="s">
         <v>12</v>
       </c>
@@ -12819,7 +12882,7 @@
       </c>
       <c r="E28" s="29"/>
       <c r="F28" s="29">
-        <f t="shared" ref="E28:H28" si="8">F24</f>
+        <f t="shared" ref="F28:H28" si="8">F24</f>
         <v>1</v>
       </c>
       <c r="G28" s="29"/>
@@ -12828,7 +12891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="27" t="s">
         <v>12</v>
       </c>
@@ -12851,7 +12914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
@@ -12878,7 +12941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="31" t="s">
         <v>15</v>
       </c>
@@ -12903,7 +12966,7 @@
       </c>
       <c r="H31" s="32"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
@@ -12930,7 +12993,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="31" t="s">
         <v>15</v>
       </c>
@@ -12957,7 +13020,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="31" t="s">
         <v>15</v>
       </c>
@@ -12989,7 +13052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="31" t="s">
         <v>15</v>
       </c>
@@ -13021,7 +13084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="31" t="s">
         <v>15</v>
       </c>
@@ -13048,7 +13111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="35" t="s">
         <v>17</v>
       </c>
@@ -13075,7 +13138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" s="35" t="s">
         <v>17</v>
       </c>
@@ -13102,7 +13165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="35" t="s">
         <v>17</v>
       </c>
@@ -13129,7 +13192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="35" t="s">
         <v>17</v>
       </c>
@@ -13156,7 +13219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" s="35" t="s">
         <v>17</v>
       </c>
@@ -13188,7 +13251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" s="35" t="s">
         <v>17</v>
       </c>
@@ -13220,7 +13283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="35" t="s">
         <v>17</v>
       </c>
@@ -13247,7 +13310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="37" t="s">
         <v>22</v>
       </c>
@@ -13274,7 +13337,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="37" t="s">
         <v>22</v>
       </c>
@@ -13301,7 +13364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="37" t="s">
         <v>22</v>
       </c>
@@ -13328,7 +13391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="37" t="s">
         <v>22</v>
       </c>
@@ -13355,7 +13418,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="37" t="s">
         <v>22</v>
       </c>
@@ -13387,7 +13450,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="37" t="s">
         <v>22</v>
       </c>
@@ -13419,7 +13482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="37" t="s">
         <v>22</v>
       </c>
@@ -13446,7 +13509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="41" t="s">
         <v>24</v>
       </c>
@@ -13473,7 +13536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="41" t="s">
         <v>24</v>
       </c>
@@ -13500,7 +13563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="41" t="s">
         <v>24</v>
       </c>
@@ -13527,7 +13590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="41" t="s">
         <v>24</v>
       </c>
@@ -13554,7 +13617,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="41" t="s">
         <v>24</v>
       </c>
@@ -13586,7 +13649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="41" t="s">
         <v>24</v>
       </c>
@@ -13618,7 +13681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="41" t="s">
         <v>24</v>
       </c>
@@ -13645,7 +13708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="45" t="s">
         <v>26</v>
       </c>
@@ -13668,7 +13731,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="45" t="s">
         <v>26</v>
       </c>
@@ -13691,7 +13754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="45" t="s">
         <v>26</v>
       </c>
@@ -13714,7 +13777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="45" t="s">
         <v>26</v>
       </c>
@@ -13737,7 +13800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="45" t="s">
         <v>26</v>
       </c>
@@ -13754,7 +13817,7 @@
       </c>
       <c r="E62" s="47"/>
       <c r="F62" s="47">
-        <f t="shared" ref="E62:H62" si="17">F58+F59+F64-$D64</f>
+        <f t="shared" ref="F62:H62" si="17">F58+F59+F64-$D64</f>
         <v>5</v>
       </c>
       <c r="G62" s="47"/>
@@ -13763,7 +13826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="45" t="s">
         <v>26</v>
       </c>
@@ -13780,7 +13843,7 @@
       </c>
       <c r="E63" s="47"/>
       <c r="F63" s="47">
-        <f t="shared" ref="E63:H63" si="18">F59</f>
+        <f t="shared" ref="F63:H63" si="18">F59</f>
         <v>4</v>
       </c>
       <c r="G63" s="47"/>
@@ -13789,7 +13852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="45" t="s">
         <v>26</v>
       </c>
@@ -13812,7 +13875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="49" t="s">
         <v>28</v>
       </c>
@@ -13839,7 +13902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="49" t="s">
         <v>28</v>
       </c>
@@ -13866,7 +13929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="49" t="s">
         <v>28</v>
       </c>
@@ -13893,7 +13956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="49" t="s">
         <v>28</v>
       </c>
@@ -13920,7 +13983,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="49" t="s">
         <v>28</v>
       </c>
@@ -13952,7 +14015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="49" t="s">
         <v>28</v>
       </c>
@@ -13984,7 +14047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="49" t="s">
         <v>28</v>
       </c>
@@ -14011,7 +14074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" s="53" t="s">
         <v>30</v>
       </c>
@@ -14038,7 +14101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" s="53" t="s">
         <v>30</v>
       </c>
@@ -14065,7 +14128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" s="53" t="s">
         <v>30</v>
       </c>
@@ -14092,7 +14155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" s="53" t="s">
         <v>30</v>
       </c>
@@ -14119,7 +14182,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" s="53" t="s">
         <v>30</v>
       </c>
@@ -14151,7 +14214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" s="53" t="s">
         <v>30</v>
       </c>
@@ -14183,7 +14246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" s="53" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
rédaction des règles (actions)
</commit_message>
<xml_diff>
--- a/Les différents types de Ferae.xlsx
+++ b/Les différents types de Ferae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bertolen\Documents\JdR\Univers\Chroniques des Ténèbres\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A49841C-3431-4128-855D-AA7E75AEA561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23A31BA-FDC3-42FF-A365-5C121E2A931A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="258">
   <si>
     <t>Espèce</t>
   </si>
@@ -521,9 +521,6 @@
   </si>
   <si>
     <t>Guérir</t>
-  </si>
-  <si>
-    <t>Ravager</t>
   </si>
   <si>
     <t>Voyager, parler</t>
@@ -1806,6 +1803,12 @@
   </si>
   <si>
     <t>Espionner</t>
+  </si>
+  <si>
+    <t>Détruire</t>
+  </si>
+  <si>
+    <t>Pestilence ?</t>
   </si>
 </sst>
 </file>
@@ -10559,7 +10562,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10589,7 +10592,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>32</v>
@@ -10598,7 +10601,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>150</v>
@@ -10610,10 +10613,10 @@
         <v>144</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>93</v>
@@ -10639,7 +10642,7 @@
         <v>151</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
@@ -10653,7 +10656,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -10676,7 +10679,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E4">
         <v>9</v>
@@ -10693,16 +10696,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" t="s">
         <v>253</v>
-      </c>
-      <c r="D5" t="s">
-        <v>254</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -10711,7 +10714,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="5"/>
@@ -10728,7 +10731,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -10740,7 +10743,7 @@
         <v>154</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>148</v>
@@ -10757,7 +10760,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -10780,7 +10783,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -10792,10 +10795,10 @@
         <v>140</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
@@ -10809,7 +10812,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -10821,7 +10824,7 @@
         <v>155</v>
       </c>
       <c r="J9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -10835,7 +10838,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -10855,7 +10858,7 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -10873,7 +10876,7 @@
         <v>149</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -10893,10 +10896,13 @@
         <v>35</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>159</v>
+        <v>256</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+      <c r="J12" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
@@ -10916,7 +10922,7 @@
         <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>92</v>
@@ -10933,7 +10939,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E14">
         <v>8</v>
@@ -10948,7 +10954,7 @@
         <v>157</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J14" t="s">
         <v>146</v>
@@ -10957,7 +10963,7 @@
         <v>145</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
@@ -11409,10 +11415,10 @@
         <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -11435,10 +11441,10 @@
         <v>38</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -11461,10 +11467,10 @@
         <v>96</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -11487,10 +11493,10 @@
         <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -11513,10 +11519,10 @@
         <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -11539,10 +11545,10 @@
         <v>50</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -11636,7 +11642,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>67</v>
@@ -11702,7 +11708,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>76</v>
@@ -11746,7 +11752,7 @@
         <v>81</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>82</v>
@@ -11849,22 +11855,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
@@ -11873,16 +11879,16 @@
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>199</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>136</v>
@@ -11897,16 +11903,16 @@
         <v>136</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>136</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="85.5" x14ac:dyDescent="0.45">
@@ -11915,16 +11921,16 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="14" t="s">
         <v>225</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>226</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>136</v>
@@ -11939,13 +11945,13 @@
         <v>136</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>136</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>136</v>
@@ -11957,16 +11963,16 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>208</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>136</v>
@@ -11977,19 +11983,19 @@
         <v>17</v>
       </c>
       <c r="B7" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="57" t="s">
         <v>237</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" s="57" t="s">
-        <v>240</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="F7" s="57" t="s">
-        <v>238</v>
       </c>
       <c r="G7" s="56" t="s">
         <v>136</v>
@@ -12004,7 +12010,7 @@
         <v>136</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>136</v>
@@ -12022,16 +12028,16 @@
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>212</v>
       </c>
       <c r="G9" s="56" t="s">
         <v>136</v>
@@ -12043,16 +12049,16 @@
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>215</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>216</v>
       </c>
       <c r="G10" s="56" t="s">
         <v>136</v>
@@ -12067,13 +12073,13 @@
         <v>136</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>136</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G11" s="56" t="s">
         <v>136</v>
@@ -12085,16 +12091,16 @@
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>222</v>
       </c>
       <c r="G12" s="56" t="s">
         <v>136</v>
@@ -12105,19 +12111,19 @@
         <v>30</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="F13" s="12" t="s">
         <v>229</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>230</v>
       </c>
       <c r="G13" s="56" t="s">
         <v>136</v>
@@ -12125,17 +12131,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="3:3" ht="57" x14ac:dyDescent="0.45">
       <c r="C19" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -12172,25 +12178,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -12202,7 +12208,7 @@
         <v>Ajaba Force</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D2" s="16">
         <v>0</v>
@@ -12229,7 +12235,7 @@
         <v>Ajaba Dextérité</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D3" s="16">
         <v>0</v>
@@ -12256,7 +12262,7 @@
         <v>Ajaba Vigueur</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="16">
         <v>0</v>
@@ -12283,7 +12289,7 @@
         <v>Ajaba Manipulation</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D5" s="16">
         <v>0</v>
@@ -12310,7 +12316,7 @@
         <v>Ajaba Vitesse</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="17">
         <f>D2+D3+D8-$D8</f>
@@ -12342,7 +12348,7 @@
         <v>Ajaba Initiative</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D7" s="17">
         <f>D3</f>
@@ -12374,7 +12380,7 @@
         <v>Ajaba Facteur espèce</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D8" s="18">
         <v>5</v>
@@ -12401,7 +12407,7 @@
         <v>Ananasi Force</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="20">
         <v>0</v>
@@ -12424,7 +12430,7 @@
         <v>Ananasi Dextérité</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" s="20">
         <v>0</v>
@@ -12447,7 +12453,7 @@
         <v>Ananasi Vigueur</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="20">
         <v>0</v>
@@ -12470,7 +12476,7 @@
         <v>Ananasi Manipulation</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D12" s="20">
         <v>0</v>
@@ -12493,7 +12499,7 @@
         <v>Ananasi Vitesse</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D13" s="21">
         <f>D9+D10+D15-$D15</f>
@@ -12522,7 +12528,7 @@
         <v>Ananasi Initiative</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D14" s="21">
         <f>D10</f>
@@ -12551,7 +12557,7 @@
         <v>Ananasi Facteur espèce</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D15" s="22">
         <v>5</v>
@@ -12576,7 +12582,7 @@
         <v>Bastet Force</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D16" s="24">
         <v>0</v>
@@ -12603,7 +12609,7 @@
         <v>Bastet Dextérité</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" s="24">
         <v>0</v>
@@ -12630,7 +12636,7 @@
         <v>Bastet Vigueur</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D18" s="24">
         <v>0</v>
@@ -12657,7 +12663,7 @@
         <v>Bastet Manipulation</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D19" s="24">
         <v>0</v>
@@ -12684,7 +12690,7 @@
         <v>Bastet Vitesse</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D20" s="25">
         <f>D16+D17+D22-$D22</f>
@@ -12716,7 +12722,7 @@
         <v>Bastet Initiative</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D21" s="25">
         <f>D17</f>
@@ -12748,7 +12754,7 @@
         <v>Bastet Facteur espèce</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D22" s="26">
         <v>5</v>
@@ -12775,7 +12781,7 @@
         <v>Corax Force</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D23" s="28">
         <v>0</v>
@@ -12798,7 +12804,7 @@
         <v>Corax Dextérité</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D24" s="28">
         <v>0</v>
@@ -12821,7 +12827,7 @@
         <v>Corax Vigueur</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" s="28">
         <v>0</v>
@@ -12844,7 +12850,7 @@
         <v>Corax Manipulation</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D26" s="28">
         <v>0</v>
@@ -12867,7 +12873,7 @@
         <v>Corax Vitesse</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D27" s="29">
         <f>D23+D24+D29-$D29</f>
@@ -12893,7 +12899,7 @@
         <v>Corax Initiative</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D28" s="29">
         <f>D24</f>
@@ -12919,7 +12925,7 @@
         <v>Corax Facteur espèce</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D29" s="30">
         <v>5</v>
@@ -12942,7 +12948,7 @@
         <v>Gurahl Force</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D30" s="32">
         <v>0</v>
@@ -12969,7 +12975,7 @@
         <v>Gurahl Dextérité</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" s="32">
         <v>0</v>
@@ -12994,7 +13000,7 @@
         <v>Gurahl Vigueur</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="32">
         <v>0</v>
@@ -13021,7 +13027,7 @@
         <v>Gurahl Manipulation</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="32">
         <v>0</v>
@@ -13048,7 +13054,7 @@
         <v>Gurahl Vitesse</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D34" s="33">
         <f>D30+D31+D36-$D36</f>
@@ -13080,7 +13086,7 @@
         <v>Gurahl Initiative</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D35" s="33">
         <f>D31</f>
@@ -13112,7 +13118,7 @@
         <v>Gurahl Facteur espèce</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D36" s="34">
         <v>5</v>
@@ -13139,7 +13145,7 @@
         <v>Kitsune Force</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D37" s="36">
         <v>0</v>
@@ -13166,7 +13172,7 @@
         <v>Kitsune Dextérité</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D38" s="36">
         <v>0</v>
@@ -13193,7 +13199,7 @@
         <v>Kitsune Vigueur</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D39" s="36">
         <v>0</v>
@@ -13220,7 +13226,7 @@
         <v>Kitsune Manipulation</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D40" s="36">
         <v>1</v>
@@ -13247,7 +13253,7 @@
         <v>Kitsune Vitesse</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D41" s="36">
         <f>D37+D38+D43-$D43</f>
@@ -13279,7 +13285,7 @@
         <v>Kitsune Initiative</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D42" s="36">
         <f>D38</f>
@@ -13311,7 +13317,7 @@
         <v>Kitsune Facteur espèce</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D43" s="36">
         <v>5</v>
@@ -13338,7 +13344,7 @@
         <v>Nâga Force</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D44" s="38">
         <v>0</v>
@@ -13365,7 +13371,7 @@
         <v>Nâga Dextérité</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D45" s="38">
         <v>0</v>
@@ -13392,7 +13398,7 @@
         <v>Nâga Vigueur</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D46" s="38">
         <v>0</v>
@@ -13419,7 +13425,7 @@
         <v>Nâga Manipulation</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D47" s="38">
         <v>0</v>
@@ -13446,7 +13452,7 @@
         <v>Nâga Vitesse</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D48" s="39">
         <f>D44+D45+D50-$D50</f>
@@ -13478,7 +13484,7 @@
         <v>Nâga Initiative</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D49" s="39">
         <f>D45</f>
@@ -13510,7 +13516,7 @@
         <v>Nâga Facteur espèce</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D50" s="40">
         <v>5</v>
@@ -13537,7 +13543,7 @@
         <v>Nuwisha Force</v>
       </c>
       <c r="C51" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D51" s="42">
         <v>0</v>
@@ -13564,7 +13570,7 @@
         <v>Nuwisha Dextérité</v>
       </c>
       <c r="C52" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D52" s="42">
         <v>0</v>
@@ -13591,7 +13597,7 @@
         <v>Nuwisha Vigueur</v>
       </c>
       <c r="C53" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D53" s="42">
         <v>0</v>
@@ -13618,7 +13624,7 @@
         <v>Nuwisha Manipulation</v>
       </c>
       <c r="C54" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D54" s="42">
         <v>0</v>
@@ -13645,7 +13651,7 @@
         <v>Nuwisha Vitesse</v>
       </c>
       <c r="C55" s="41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D55" s="43">
         <f>D51+D52+D57-$D57</f>
@@ -13677,7 +13683,7 @@
         <v>Nuwisha Initiative</v>
       </c>
       <c r="C56" s="41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D56" s="43">
         <f>D52</f>
@@ -13709,7 +13715,7 @@
         <v>Nuwisha Facteur espèce</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D57" s="44">
         <v>5</v>
@@ -13736,7 +13742,7 @@
         <v>Ratkin Force</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D58" s="46">
         <v>0</v>
@@ -13759,7 +13765,7 @@
         <v>Ratkin Dextérité</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D59" s="46">
         <v>0</v>
@@ -13782,7 +13788,7 @@
         <v>Ratkin Vigueur</v>
       </c>
       <c r="C60" s="45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D60" s="46">
         <v>0</v>
@@ -13805,7 +13811,7 @@
         <v>Ratkin Manipulation</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D61" s="46">
         <v>0</v>
@@ -13828,7 +13834,7 @@
         <v>Ratkin Vitesse</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D62" s="47">
         <f>D58+D59+D64-$D64</f>
@@ -13854,7 +13860,7 @@
         <v>Ratkin Initiative</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D63" s="47">
         <f>D59</f>
@@ -13880,7 +13886,7 @@
         <v>Ratkin Facteur espèce</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D64" s="48">
         <v>5</v>
@@ -13903,7 +13909,7 @@
         <v>Rokea Force</v>
       </c>
       <c r="C65" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D65" s="50">
         <v>0</v>
@@ -13930,7 +13936,7 @@
         <v>Rokea Dextérité</v>
       </c>
       <c r="C66" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D66" s="50">
         <v>0</v>
@@ -13957,7 +13963,7 @@
         <v>Rokea Vigueur</v>
       </c>
       <c r="C67" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D67" s="50">
         <v>0</v>
@@ -13984,7 +13990,7 @@
         <v>Rokea Manipulation</v>
       </c>
       <c r="C68" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D68" s="50">
         <v>0</v>
@@ -14011,7 +14017,7 @@
         <v>Rokea Vitesse</v>
       </c>
       <c r="C69" s="49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D69" s="51">
         <f>D65+D66+D71-$D71</f>
@@ -14043,7 +14049,7 @@
         <v>Rokea Initiative</v>
       </c>
       <c r="C70" s="49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D70" s="51">
         <f>D66</f>
@@ -14075,7 +14081,7 @@
         <v>Rokea Facteur espèce</v>
       </c>
       <c r="C71" s="49" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D71" s="52">
         <v>5</v>
@@ -14102,7 +14108,7 @@
         <v>Uratha Force</v>
       </c>
       <c r="C72" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D72" s="54">
         <v>0</v>
@@ -14129,7 +14135,7 @@
         <v>Uratha Dextérité</v>
       </c>
       <c r="C73" s="53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D73" s="54">
         <v>0</v>
@@ -14156,7 +14162,7 @@
         <v>Uratha Vigueur</v>
       </c>
       <c r="C74" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D74" s="54">
         <v>0</v>
@@ -14183,7 +14189,7 @@
         <v>Uratha Manipulation</v>
       </c>
       <c r="C75" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D75" s="54">
         <v>0</v>
@@ -14210,7 +14216,7 @@
         <v>Uratha Vitesse</v>
       </c>
       <c r="C76" s="53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D76" s="54">
         <f>D72+D73+D78-$D78</f>
@@ -14242,7 +14248,7 @@
         <v>Uratha Initiative</v>
       </c>
       <c r="C77" s="53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D77" s="54">
         <f>D73</f>
@@ -14274,7 +14280,7 @@
         <v>Uratha Facteur espèce</v>
       </c>
       <c r="C78" s="53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D78" s="54">
         <v>5</v>

</xml_diff>